<commit_message>
Redesigned & Improved the students exam  modal
</commit_message>
<xml_diff>
--- a/CLASS/SS2/Accounting/results.xlsx
+++ b/CLASS/SS2/Accounting/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,6 +554,49 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>AbdulHafiz Ismail Mambo</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>std272</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SS2_SILVER</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ACCOUNTING</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>16%</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" t="n">
+        <v>50</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>FAIL</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2025-12-06 18:28</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>